<commit_message>
upd docs, added owl params
</commit_message>
<xml_diff>
--- a/tables/bachelors/4th_course/Cтуденты 2022-2023 уч. год.xlsx
+++ b/tables/bachelors/4th_course/Cтуденты 2022-2023 уч. год.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="495" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-105" yWindow="495" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Практика 3 к. бак." sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3237" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3254" uniqueCount="325">
   <si>
     <t>ФИО студента</t>
   </si>
@@ -925,9 +925,6 @@
   </si>
   <si>
     <t>Павлов Евгений Александрович</t>
-  </si>
-  <si>
-    <t>с.н.с. НОЦГПН</t>
   </si>
   <si>
     <t>Производственная практика, преддипломная практика</t>
@@ -1513,6 +1510,42 @@
   </si>
   <si>
     <t>зам. директора</t>
+  </si>
+  <si>
+    <t>Инициалы</t>
+  </si>
+  <si>
+    <t>Вишневский О.В.</t>
+  </si>
+  <si>
+    <t>Барахнин В.Б.</t>
+  </si>
+  <si>
+    <t>Пальчунов Д.Е.</t>
+  </si>
+  <si>
+    <t>Савостьянов А.Н.</t>
+  </si>
+  <si>
+    <t>Хазанкин Г.Р.</t>
+  </si>
+  <si>
+    <t>Дучков А.А.</t>
+  </si>
+  <si>
+    <t>Марчук А.Г.</t>
+  </si>
+  <si>
+    <t>Свириденко Д.И.</t>
+  </si>
+  <si>
+    <t>Добрецов Н.Н.</t>
+  </si>
+  <si>
+    <t>Яскевич С.В.</t>
+  </si>
+  <si>
+    <t>Дудкин Ф.А.</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1619,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1602,12 +1635,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1667,7 +1694,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1720,9 +1747,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2964,7 +2988,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -3076,7 +3100,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -3132,7 +3156,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>61</v>
       </c>
@@ -3188,7 +3212,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>62</v>
       </c>
@@ -3244,7 +3268,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>63</v>
       </c>
@@ -3300,7 +3324,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>49</v>
       </c>
@@ -3468,7 +3492,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
@@ -3580,7 +3604,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
@@ -3636,7 +3660,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
@@ -3692,7 +3716,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -3748,7 +3772,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>72</v>
       </c>
@@ -3804,7 +3828,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
@@ -3860,7 +3884,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>11</v>
       </c>
@@ -3916,7 +3940,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>51</v>
       </c>
@@ -3972,7 +3996,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
@@ -4028,7 +4052,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>52</v>
       </c>
@@ -4084,7 +4108,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
@@ -4140,7 +4164,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -4196,7 +4220,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>53</v>
       </c>
@@ -4252,7 +4276,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>65</v>
       </c>
@@ -4364,7 +4388,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>67</v>
       </c>
@@ -4420,7 +4444,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>68</v>
       </c>
@@ -4476,7 +4500,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>20</v>
       </c>
@@ -4532,7 +4556,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>21</v>
       </c>
@@ -4588,7 +4612,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>22</v>
       </c>
@@ -4644,7 +4668,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>23</v>
       </c>
@@ -4700,7 +4724,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>73</v>
       </c>
@@ -4756,7 +4780,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -4812,7 +4836,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
@@ -4868,7 +4892,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>24</v>
       </c>
@@ -4924,7 +4948,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>13</v>
       </c>
@@ -4980,7 +5004,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>69</v>
       </c>
@@ -5036,7 +5060,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>25</v>
       </c>
@@ -5092,7 +5116,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>74</v>
       </c>
@@ -5204,7 +5228,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>75</v>
       </c>
@@ -5260,7 +5284,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>26</v>
       </c>
@@ -5316,7 +5340,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>27</v>
       </c>
@@ -5372,7 +5396,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>76</v>
       </c>
@@ -5428,7 +5452,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>28</v>
       </c>
@@ -5484,7 +5508,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>29</v>
       </c>
@@ -5540,7 +5564,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>70</v>
       </c>
@@ -5596,7 +5620,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>71</v>
       </c>
@@ -5764,7 +5788,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>12</v>
       </c>
@@ -5820,7 +5844,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>37</v>
       </c>
@@ -5876,7 +5900,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>30</v>
       </c>
@@ -5932,7 +5956,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>56</v>
       </c>
@@ -5988,7 +6012,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
@@ -6044,7 +6068,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>7</v>
       </c>
@@ -6119,8 +6143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6201,7 +6225,7 @@
         <v>219</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>6</v>
@@ -6243,7 +6267,7 @@
         <v>260</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6257,7 +6281,7 @@
         <v>220</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>84</v>
@@ -6299,7 +6323,7 @@
         <v>260</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6313,7 +6337,7 @@
         <v>220</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>60</v>
@@ -6355,7 +6379,7 @@
         <v>260</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6369,7 +6393,7 @@
         <v>221</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>88</v>
@@ -6411,7 +6435,7 @@
         <v>260</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6425,7 +6449,7 @@
         <v>222</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>6</v>
@@ -6467,7 +6491,7 @@
         <v>260</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6481,7 +6505,7 @@
         <v>219</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>88</v>
@@ -6523,7 +6547,7 @@
         <v>260</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6537,7 +6561,7 @@
         <v>220</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>39</v>
@@ -6575,7 +6599,7 @@
         <v>260</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6589,7 +6613,7 @@
         <v>220</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>39</v>
@@ -6631,7 +6655,7 @@
         <v>260</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6645,7 +6669,7 @@
         <v>223</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>84</v>
@@ -6687,7 +6711,7 @@
         <v>260</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6701,7 +6725,7 @@
         <v>224</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>39</v>
@@ -6743,7 +6767,7 @@
         <v>260</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6757,7 +6781,7 @@
         <v>223</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>9</v>
@@ -6799,7 +6823,7 @@
         <v>260</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6813,7 +6837,7 @@
         <v>219</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>6</v>
@@ -6855,7 +6879,7 @@
         <v>260</v>
       </c>
       <c r="R13" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6869,7 +6893,7 @@
         <v>225</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>102</v>
@@ -6911,7 +6935,7 @@
         <v>260</v>
       </c>
       <c r="R14" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6925,7 +6949,7 @@
         <v>220</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>39</v>
@@ -6967,7 +6991,7 @@
         <v>260</v>
       </c>
       <c r="R15" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -6981,7 +7005,7 @@
         <v>222</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>88</v>
@@ -7023,7 +7047,7 @@
         <v>260</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7037,7 +7061,7 @@
         <v>220</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>39</v>
@@ -7079,7 +7103,7 @@
         <v>260</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7093,7 +7117,7 @@
         <v>220</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>39</v>
@@ -7135,7 +7159,7 @@
         <v>260</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7149,7 +7173,7 @@
         <v>222</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>6</v>
@@ -7191,7 +7215,7 @@
         <v>260</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7205,7 +7229,7 @@
         <v>219</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>88</v>
@@ -7247,7 +7271,7 @@
         <v>260</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7261,7 +7285,7 @@
         <v>227</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>60</v>
@@ -7303,7 +7327,7 @@
         <v>260</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7317,7 +7341,7 @@
         <v>222</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>60</v>
@@ -7359,7 +7383,7 @@
         <v>260</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7373,7 +7397,7 @@
         <v>226</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>60</v>
@@ -7415,7 +7439,7 @@
         <v>260</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7429,7 +7453,7 @@
         <v>221</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>102</v>
@@ -7471,7 +7495,7 @@
         <v>260</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7485,7 +7509,7 @@
         <v>221</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>88</v>
@@ -7527,7 +7551,7 @@
         <v>260</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7541,7 +7565,7 @@
         <v>224</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>82</v>
@@ -7559,29 +7583,29 @@
       <c r="J26" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K26" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="L26" s="20" t="s">
+      <c r="K26" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="L26" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="M26" s="20" t="s">
+      <c r="M26" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="N26" s="20" t="s">
+      <c r="N26" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="O26" s="20" t="s">
+      <c r="O26" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="P26" s="20" t="s">
+      <c r="P26" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="Q26" s="20" t="s">
+      <c r="Q26" s="17" t="s">
         <v>266</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7595,7 +7619,7 @@
         <v>227</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>60</v>
@@ -7637,7 +7661,7 @@
         <v>260</v>
       </c>
       <c r="R27" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7651,7 +7675,7 @@
         <v>219</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>60</v>
@@ -7693,7 +7717,7 @@
         <v>260</v>
       </c>
       <c r="R28" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7707,7 +7731,7 @@
         <v>222</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>102</v>
@@ -7749,7 +7773,7 @@
         <v>260</v>
       </c>
       <c r="R29" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7763,7 +7787,7 @@
         <v>228</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>88</v>
@@ -7801,7 +7825,7 @@
         <v>260</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7815,7 +7839,7 @@
         <v>227</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>84</v>
@@ -7857,7 +7881,7 @@
         <v>260</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7871,7 +7895,7 @@
         <v>220</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>6</v>
@@ -7913,7 +7937,7 @@
         <v>260</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7927,7 +7951,7 @@
         <v>228</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>39</v>
@@ -7969,7 +7993,7 @@
         <v>260</v>
       </c>
       <c r="R33" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -7983,7 +8007,7 @@
         <v>224</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>6</v>
@@ -8025,7 +8049,7 @@
         <v>260</v>
       </c>
       <c r="R34" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8039,7 +8063,7 @@
         <v>222</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>84</v>
@@ -8081,7 +8105,7 @@
         <v>260</v>
       </c>
       <c r="R35" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8095,7 +8119,7 @@
         <v>228</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E36" s="17" t="s">
         <v>80</v>
@@ -8137,7 +8161,7 @@
         <v>266</v>
       </c>
       <c r="R36" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8151,7 +8175,7 @@
         <v>225</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E37" s="17" t="s">
         <v>82</v>
@@ -8193,7 +8217,7 @@
         <v>266</v>
       </c>
       <c r="R37" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8207,7 +8231,7 @@
         <v>225</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>80</v>
@@ -8249,7 +8273,7 @@
         <v>266</v>
       </c>
       <c r="R38" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8263,7 +8287,7 @@
         <v>224</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>80</v>
@@ -8305,7 +8329,7 @@
         <v>266</v>
       </c>
       <c r="R39" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8319,7 +8343,7 @@
         <v>225</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E40" s="17" t="s">
         <v>82</v>
@@ -8361,7 +8385,7 @@
         <v>266</v>
       </c>
       <c r="R40" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8375,7 +8399,7 @@
         <v>225</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E41" s="17" t="s">
         <v>82</v>
@@ -8417,7 +8441,7 @@
         <v>266</v>
       </c>
       <c r="R41" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8431,7 +8455,7 @@
         <v>228</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E42" s="17" t="s">
         <v>84</v>
@@ -8446,7 +8470,7 @@
         <v>266</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J42" s="17" t="s">
         <v>84</v>
@@ -8473,7 +8497,7 @@
         <v>260</v>
       </c>
       <c r="R42" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8487,7 +8511,7 @@
         <v>225</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E43" s="17" t="s">
         <v>80</v>
@@ -8529,7 +8553,7 @@
         <v>266</v>
       </c>
       <c r="R43" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8543,7 +8567,7 @@
         <v>223</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>32</v>
@@ -8585,7 +8609,7 @@
         <v>260</v>
       </c>
       <c r="R44" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8599,7 +8623,7 @@
         <v>220</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>32</v>
@@ -8641,7 +8665,7 @@
         <v>260</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8655,7 +8679,7 @@
         <v>227</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E46" s="17" t="s">
         <v>32</v>
@@ -8697,7 +8721,7 @@
         <v>260</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8711,7 +8735,7 @@
         <v>227</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>32</v>
@@ -8753,7 +8777,7 @@
         <v>260</v>
       </c>
       <c r="R47" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8767,7 +8791,7 @@
         <v>225</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E48" s="17" t="s">
         <v>9</v>
@@ -8809,7 +8833,7 @@
         <v>266</v>
       </c>
       <c r="R48" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -8823,7 +8847,7 @@
         <v>223</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E49" s="17" t="s">
         <v>2</v>
@@ -8865,12 +8889,12 @@
         <v>260</v>
       </c>
       <c r="R49" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>191</v>
@@ -8879,7 +8903,7 @@
         <v>224</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E50" s="17" t="s">
         <v>84</v>
@@ -8892,7 +8916,7 @@
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J50" s="17" t="s">
         <v>84</v>
@@ -8917,12 +8941,12 @@
         <v>260</v>
       </c>
       <c r="R50" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>191</v>
@@ -8931,7 +8955,7 @@
         <v>222</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E51" s="17" t="s">
         <v>2</v>
@@ -8973,7 +8997,7 @@
         <v>260</v>
       </c>
       <c r="R51" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -10795,7 +10819,7 @@
         <v>260</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>209</v>
@@ -10825,7 +10849,7 @@
         <v>260</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10851,7 +10875,7 @@
         <v>260</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>194</v>
@@ -10881,7 +10905,7 @@
         <v>260</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10907,7 +10931,7 @@
         <v>260</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>194</v>
@@ -10937,7 +10961,7 @@
         <v>260</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10963,7 +10987,7 @@
         <v>260</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>194</v>
@@ -10993,7 +11017,7 @@
         <v>260</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11019,7 +11043,7 @@
         <v>260</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>209</v>
@@ -11049,7 +11073,7 @@
         <v>260</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11075,7 +11099,7 @@
         <v>266</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>248</v>
@@ -11105,7 +11129,7 @@
         <v>266</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11131,7 +11155,7 @@
         <v>260</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>249</v>
@@ -11161,7 +11185,7 @@
         <v>266</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11187,7 +11211,7 @@
         <v>260</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>194</v>
@@ -11217,7 +11241,7 @@
         <v>260</v>
       </c>
       <c r="R9" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11243,7 +11267,7 @@
         <v>260</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>194</v>
@@ -11273,7 +11297,7 @@
         <v>260</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11299,7 +11323,7 @@
         <v>260</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>194</v>
@@ -11329,7 +11353,7 @@
         <v>260</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11355,7 +11379,7 @@
         <v>266</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>248</v>
@@ -11385,7 +11409,7 @@
         <v>266</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11411,7 +11435,7 @@
         <v>260</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>194</v>
@@ -11441,7 +11465,7 @@
         <v>260</v>
       </c>
       <c r="R13" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11467,7 +11491,7 @@
         <v>260</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>194</v>
@@ -11497,7 +11521,7 @@
         <v>260</v>
       </c>
       <c r="R14" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="110.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11523,7 +11547,7 @@
         <v>266</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>207</v>
@@ -11553,7 +11577,7 @@
         <v>260</v>
       </c>
       <c r="R15" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -11572,7 +11596,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11937,7 +11961,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12234,10 +12258,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12246,7 +12270,7 @@
     <col min="2" max="16384" width="23.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>252</v>
       </c>
@@ -12262,8 +12286,11 @@
       <c r="E1" s="7" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -12279,8 +12306,11 @@
       <c r="E2" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>217</v>
       </c>
@@ -12296,8 +12326,11 @@
       <c r="E3" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -12313,8 +12346,11 @@
       <c r="E4" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -12330,8 +12366,11 @@
       <c r="E5" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>266</v>
       </c>
@@ -12348,7 +12387,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>202</v>
       </c>
@@ -12364,16 +12403,19 @@
       <c r="E7" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>262</v>
@@ -12381,8 +12423,11 @@
       <c r="E8" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>166</v>
       </c>
@@ -12398,8 +12443,11 @@
       <c r="E9" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>139</v>
       </c>
@@ -12415,8 +12463,11 @@
       <c r="E10" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>250</v>
       </c>
@@ -12432,8 +12483,11 @@
       <c r="E11" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>82</v>
       </c>
@@ -12445,6 +12499,29 @@
       </c>
       <c r="D12" s="2" t="s">
         <v>262</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>